<commit_message>
Excel cinverter added. Explorer bug fixed. On paypal closed added javascript to redirect to result tab. Chrome bug fixed duble click issue.
</commit_message>
<xml_diff>
--- a/public/nfs-share/4/csv/Book1.xlsx
+++ b/public/nfs-share/4/csv/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>user1</t>
   </si>
@@ -57,61 +57,53 @@
     <t>user13</t>
   </si>
   <si>
-    <t>user1@mail.com</t>
-  </si>
-  <si>
-    <t>0544464204</t>
-  </si>
-  <si>
-    <t>0544464205</t>
-  </si>
-  <si>
-    <t>0544464206</t>
-  </si>
-  <si>
-    <t>0544464207</t>
-  </si>
-  <si>
-    <t>0544464208</t>
-  </si>
-  <si>
-    <t>0544464209</t>
-  </si>
-  <si>
-    <t>0544464210</t>
-  </si>
-  <si>
-    <t>0544464211</t>
-  </si>
-  <si>
-    <t>0544464212</t>
-  </si>
-  <si>
-    <t>0544464213</t>
-  </si>
-  <si>
-    <t>0544464214</t>
-  </si>
-  <si>
-    <t>0544464215</t>
+    <t>054-4464204</t>
+  </si>
+  <si>
+    <t>054-4464205</t>
+  </si>
+  <si>
+    <t>054-4464206</t>
+  </si>
+  <si>
+    <t>054-4464207</t>
+  </si>
+  <si>
+    <t>054-4464208</t>
+  </si>
+  <si>
+    <t>054-4464209</t>
+  </si>
+  <si>
+    <t>054-4464210</t>
+  </si>
+  <si>
+    <t>054-4464211</t>
+  </si>
+  <si>
+    <t>054-4464212</t>
+  </si>
+  <si>
+    <t>054-4464213</t>
+  </si>
+  <si>
+    <t>054-4464214</t>
+  </si>
+  <si>
+    <t>054-4464215</t>
+  </si>
+  <si>
+    <t>054-4464216</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,17 +126,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,168 +433,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B2:B13" r:id="rId2" display="user1@mail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>